<commit_message>
Emry, Leovold and Narset added to decklists
</commit_message>
<xml_diff>
--- a/Datos/Decklists.xlsx
+++ b/Datos/Decklists.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A54EB7A-EC75-422A-96B2-5F9E3BB6D741}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAA9F6B-2ACB-40A4-BAD1-17F4AE813707}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="8925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,9 +106,6 @@
     <t>Selfless Spirit</t>
   </si>
   <si>
-    <t>Lena, Slefless Champion</t>
-  </si>
-  <si>
     <t>Akiri, Fearless Voyager</t>
   </si>
   <si>
@@ -157,9 +154,6 @@
     <t>Mana Crypt</t>
   </si>
   <si>
-    <t>Dockside Extorsionist</t>
-  </si>
-  <si>
     <t>Legion's Landing</t>
   </si>
   <si>
@@ -223,9 +217,6 @@
     <t>Sol Ring</t>
   </si>
   <si>
-    <t>Mortapod</t>
-  </si>
-  <si>
     <t>Command Tower</t>
   </si>
   <si>
@@ -302,6 +293,15 @@
   </si>
   <si>
     <t>Wooded Foothills</t>
+  </si>
+  <si>
+    <t>Mortarpod</t>
+  </si>
+  <si>
+    <t>Dockside Extortionist</t>
+  </si>
+  <si>
+    <t>Lena, Selfless Champion</t>
   </si>
 </sst>
 </file>
@@ -649,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,362 +800,362 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>